<commit_message>
Added rules to implement simplified pseudonymization and field removal (see todo items 1 and 2)
</commit_message>
<xml_diff>
--- a/sampleData/characters-invalid.xlsx
+++ b/sampleData/characters-invalid.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>110a</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
+    <t>Peggy Hill</t>
+  </si>
+  <si>
+    <t>Marge Simpson</t>
   </si>
 </sst>
 </file>
@@ -381,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,9 +401,10 @@
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,8 +417,11 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -421,8 +434,11 @@
       <c r="D2">
         <v>220</v>
       </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -433,7 +449,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -447,7 +463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -459,6 +475,9 @@
       </c>
       <c r="D5">
         <v>235</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifications to sample data to make them more useful
</commit_message>
<xml_diff>
--- a/sampleData/characters-invalid.xlsx
+++ b/sampleData/characters-invalid.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Hank Hill</t>
   </si>
   <si>
-    <t>Eric Carman</t>
-  </si>
-  <si>
     <t>Elmer Fudd</t>
   </si>
   <si>
@@ -52,6 +49,12 @@
   </si>
   <si>
     <t>Marge Simpson</t>
+  </si>
+  <si>
+    <t>Eric Cartman</t>
+  </si>
+  <si>
+    <t>Homer J. Simpson</t>
   </si>
 </sst>
 </file>
@@ -390,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,13 +415,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -435,12 +438,12 @@
         <v>220</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>38</v>
@@ -451,33 +454,67 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="C4">
-        <v>61</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+        <v>66</v>
+      </c>
+      <c r="D4">
+        <v>125</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
+        <v>79</v>
+      </c>
+      <c r="C5">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>43</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>68</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>235</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>43</v>
+      </c>
+      <c r="C7">
+        <v>78</v>
+      </c>
+      <c r="D7">
+        <v>135</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>